<commit_message>
ending wiht chd lmc gamma and normal
</commit_message>
<xml_diff>
--- a/chd_lmc_gamma/chd_grid_Q_Normal.xlsx
+++ b/chd_lmc_gamma/chd_grid_Q_Normal.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,142 +462,162 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B2" t="n">
-        <v>-52.11076836408649</v>
+        <v>-49.8303533733402</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.425749241060391</v>
+        <v>-1.285958296698702</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03084369641434469</v>
+        <v>0.03012870743856047</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01519486422716895</v>
+        <v>0.002715833562876155</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02952935479515713</v>
+        <v>0.03149110810101963</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>-50.54679044263008</v>
+        <v>-44.45422979399342</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.33711844151089</v>
+        <v>-0.9429480844145793</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06628007048084651</v>
+        <v>0.03727361920264568</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002609949250685696</v>
+        <v>0.004112031532115542</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03102956711975482</v>
+        <v>0.0389895444232617</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B4" t="n">
-        <v>-49.79321383569138</v>
+        <v>-49.12644518608512</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.297030706907894</v>
+        <v>-1.234518913264335</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05807541702330681</v>
+        <v>0.08183332923410236</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002678976258912376</v>
+        <v>0.002938813338652266</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03196817446861536</v>
+        <v>0.03307793574342761</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B5" t="n">
-        <v>-49.79910892519096</v>
+        <v>-49.08736175233031</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.298239523144986</v>
+        <v>-1.262833530135628</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0593746368836556</v>
+        <v>0.03039696420631934</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00301729476388712</v>
+        <v>0.002849600249672071</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03159177579430397</v>
+        <v>0.03176445169193558</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B6" t="n">
-        <v>-51.43861276450299</v>
+        <v>-48.72457008755512</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.387952461402734</v>
+        <v>-1.204407234879717</v>
       </c>
       <c r="D6" t="n">
-        <v>37623.85213186133</v>
+        <v>0.03203233451463891</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0242539667340785</v>
+        <v>0.003057073877455373</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0474812788956409</v>
+        <v>0.03426768450626295</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B7" t="n">
-        <v>-53.71219871580401</v>
+        <v>-42.10659406711788</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.510758625405628</v>
+        <v>-0.8375361046424108</v>
       </c>
       <c r="D7" t="n">
-        <v>1038952472.840376</v>
+        <v>0.04028077999362526</v>
       </c>
       <c r="E7" t="n">
-        <v>265.8197050283166</v>
+        <v>0.004487459974258948</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5889318867024346</v>
+        <v>0.04242369853510088</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B8" t="n">
-        <v>-47.14438594595703</v>
+        <v>-50.74085032341767</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.102674194672744</v>
+        <v>-1.35207691598998</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03372530005278603</v>
+        <v>0.05923577998107189</v>
       </c>
       <c r="E8" t="n">
-        <v>0.003443571725550474</v>
+        <v>0.002453689080871777</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03522314297920232</v>
+        <v>0.03743885377620029</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-43.85653625902743</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.9193241304295263</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.03756831901965291</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.004167149281924271</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.03937916771150821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>